<commit_message>
Added roll macro to conditions and variable management, added contains test and Array Variables.
</commit_message>
<xml_diff>
--- a/Ressources/Test/Story.xlsx
+++ b/Ressources/Test/Story.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="79">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -55,7 +55,8 @@
 PAR003:To the mountains;</t>
   </si>
   <si>
-    <t xml:space="preserve">MUSIC:timbre__logicmoons-freesound.ogg</t>
+    <t xml:space="preserve">MUSIC:timbre__logicmoons-freesound.ogg;
+SET:Hero.Intelligence:[2d6];</t>
   </si>
   <si>
     <t xml:space="preserve">TEXTONLY</t>
@@ -77,7 +78,13 @@
     <t xml:space="preserve">PAR003</t>
   </si>
   <si>
-    <t xml:space="preserve">The mountain is too steep, and you die from fallen stones.</t>
+    <t xml:space="preserve">Your ascension leads to a crossway. With no better indications, you roll a dice and continue your journey on the designated tracks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SET:W.buffer:[1d6];
+IF:W.buffer&lt;=2;CHOICE:PAR012:You go to the left.;
+IF:W.buffer&gt;=5;CHOICE:PAR013:You go to the right.;
+CHOICE:PAR014:You continue straight forward.</t>
   </si>
   <si>
     <t xml:space="preserve">PAR004</t>
@@ -151,6 +158,143 @@
   <si>
     <t xml:space="preserve">You are helpless ! Falling in the dark, your downfall knows no end, no witness. Your dead body will not be found before years.
 Here ends your journey.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The road if full of rocks, and dust, following the top of a cliff. When suddenly, your eye catches the glimpse of fire from a under a rock at your feet.
+With care, you set the stone aside, and reveal a flamboyant metal ring, glimmering with iridescent reflects. Captivated by its lights, you decide to keep it at your finger.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD[]:Hero.Equipement:Red Ring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After a long walk, you arrive at what seems like a small temple. Ripped trees, the wood seemingly burned by fire, are scattered through what would have otherwise be a refreshing orchard. On the right, a small storage, the door left open. On the center, the main temple, of marble steps and pillars. The roof is loaded with red tiles and withered vines. The inside, hidden from the sunlight, seems awfully quiet, and you can hear not a single bird chirping in the valley.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR015:Explore the small storage.;
+PAR016:Explore the burned orchard.;
+PAR018:Go straight to the temple.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The path is steep, bushes grip to your clothes, and the wind is pushing you to the side. In order to reach to peak of the mountain, you have no other choice but to start climbing to cliffs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF:Hero.Intelligence&gt;=[2d6];
+CHOICE:PAR021;
+CHOICE:PAR017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This small house is a storehouse for broken and unused goods, heaped without any apparent logic. You advance slowly among the dust and the spiderwebs, when you notice some footsteps leading behind some barrels. Here, you discover a terrified child, hunched under a filthy blanket. At your sight, he yells of relieve. “You are alive ! Is everyone alright ?” But you can only put your ignorance on display, and ask for what happened. The boy seems to fall in panic again. “The djinn ! The master said it was a djinn. He is looking for something, but the master he must not find it.” You press the child with questions, but he doesn’t seem to know much more, and his explanations lack clarity. All you manage to understand is that a malevolent djinn had attacked the temple and slaughtered everyone in his quest for a powerful item. Maybe you should investigate more.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR018:Go back and head to the temple.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD[]:W.Places:15;
+CONTAINS:W.Places:16;;CHOICE:PAR016:Go back and explore the orchard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You walk slowly into the orchard. The dirt and the ash crackling under your feet. At first, you hear nothing, you see nothing. But suddenly behind a tree you notice a gloom heap of burned corpses, animals and humans alike, all blackened and left dry by the intense fire that must have killed them. There is nothing more to be seen here. You leave this place at once, the mind shaken by this horrible sight.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD[]:W.Flags:16;
+ADD:Hero.Intelligence:-1;
+CONTAINS:W.Flags:15;;CHOICE:PAR015:Go back and explore the small storage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What a fool you are ! The mountain is too steep, and you die from fallen stones.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You enter the white halls with caution. Stains of ash and blood are everywhere to be seen. A scream of fear and suffering draws your attention, and you rush towards it. Here, a giant man, shirtless, the skin red like fresh blood, long black hair tied to the back of his head, lifts a man up in the air by the throat. Before you have the time to do anything, he clenches his fist, and the man’s eyes roll back into his head, in the midst of gurgling throat and crushed bones.
+And only then the giant turns towards you in face with an intense satisfaction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTAINS:Hero.Equipement:Red Ring;
+CHOICE:PAR019;
+CHOICE:PAR020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The red giant sees the ring of fire colors at your finger, and turns all his attention towards you, a spark of hatred in the eye.
+“You have what belongs to me!”, he says. His deep voice reverberating in the vast marble halls. “Give it back to me, and I will spare your miserable life. May you be foolish enough to decline my kind offer, and I will throw you into the maws of the great Etna, where sulfur and fire will consume the best of you.” </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR022:Give the ring;
+PAR023:Refuse;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF:Hero.Intelligence&gt;=9;CHOICE:PAR024:[INT] Throw the ring away.;;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The giant approaches you and rise his menacing sword, leaving you no other choice than battle. But beware of the flames dancing around him. At each assault, roll a die. On a 1,2, or 3, you loose 2 Stamina.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMBAT:Red Giant,11,13:-1:;
+IF:[1d6]&lt;=3;ADD:Hero.Current.Stamina:-2;;
+CHOICE:PAR025;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You finally reach the summit of the mountain, and after a quick breath, starts your descent into the valley at your feet.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You don’t have much choice. You remove the ring from your finger, and hand it to the giant. “Ha, the singing of forged steel wringing under the blazing fire! What a sweet ringing to my ears !” He says while grasping the ring violently from your hand. “After all this centuries, finally I have found you ! And for you, you have all my gratitude. I will make your death quick and painless.”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REM[]:Hero.Equipement:Red Ring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR023</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Refuse to give the ring # Confrontation with the ring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMBAT:Red Giant,9,13:-1:;
+IF:[1d6]&lt;=3;ADD:Hero.Current.Stamina:1;;
+CHOICE:PAR025;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR024</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Throwing the ring away behind the giant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAR025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Djinn victory</t>
   </si>
 </sst>
 </file>
@@ -160,7 +304,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -199,6 +343,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="128"/>
     </font>
@@ -251,7 +402,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -270,6 +421,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -524,18 +683,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.69140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="54.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="40.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="46.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.98"/>
   </cols>
   <sheetData>
@@ -559,7 +718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="38" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -572,7 +731,7 @@
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -593,88 +752,252 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="38" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="74" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="98" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="62" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="38" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="38" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="62" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="74" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="41" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="38" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="38" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="38" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="26" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="38" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="38" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>